<commit_message>
update after Amen comment
Edit testcases in OnboardTask_001.xlsx

Use Hooks, POM, Lazy initialization pattern. split one file(AccountProfile) to 8 Pages files and 7 stepDefinition file.
</commit_message>
<xml_diff>
--- a/OnboardTask_002.xlsx
+++ b/OnboardTask_002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\IndustryConnect\Day24Week8OnboardingTask\Day24Week8OnboardingTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C66FB2-0B41-4942-8FFD-6910F43816FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDF39CE-12C6-4AE7-98CC-F0C9C65C17F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{E9E6E289-72CB-45F8-8006-5355E1426F22}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Cases'!$A$1:$AD$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
   <si>
     <t>User Story 1:</t>
   </si>
@@ -264,12 +265,6 @@
 4 click add</t>
   </si>
   <si>
-    <t>1 select add new language
-2 fill many pharagraph on language field
-3 choose language level
-4 click add</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 select add new language
 2 fill a language
 3 choose language level
@@ -399,9 +394,6 @@
   </si>
   <si>
     <t>TS_100_TC_006 Verify that the user add a new Languages on the account profile page with duplicate on Add Language field</t>
-  </si>
-  <si>
-    <t>TS_100_TC_007 Verify that the user add a new Languages on the account profile page with many paragraph on Add Language field</t>
   </si>
   <si>
     <t>TS_100_TC_008 Verify that the user add new 4 Languages on the account profile page with a paragraph on Add Language field</t>
@@ -651,6 +643,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -661,9 +656,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1053,11 +1045,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8EC9D0-C91D-48DD-971A-EE0308A56452}">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,14 +1124,14 @@
       <c r="AD1" s="2"/>
     </row>
     <row r="2" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>85</v>
+      <c r="C2" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>26</v>
@@ -1167,10 +1159,10 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="21" t="s">
-        <v>86</v>
+      <c r="A3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>26</v>
@@ -1198,10 +1190,10 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21" t="s">
-        <v>87</v>
+      <c r="A4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>26</v>
@@ -1213,7 +1205,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="13" t="s">
@@ -1225,10 +1217,10 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="21" t="s">
-        <v>88</v>
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>26</v>
@@ -1240,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="13" t="s">
@@ -1252,10 +1244,10 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="21" t="s">
-        <v>89</v>
+      <c r="A6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>26</v>
@@ -1267,7 +1259,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="13" t="s">
@@ -1279,22 +1271,22 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="21" t="s">
-        <v>90</v>
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="13" t="s">
@@ -1306,10 +1298,10 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="21" t="s">
-        <v>91</v>
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
@@ -1321,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="13" t="s">
@@ -1329,14 +1321,14 @@
       </c>
       <c r="J8" s="13"/>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="21" t="s">
-        <v>92</v>
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>26</v>
@@ -1348,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="13" t="s">
@@ -1360,70 +1352,70 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21" t="s">
-        <v>93</v>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="12"/>
+        <v>54</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="13"/>
+      <c r="J10" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>94</v>
+      <c r="A11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="H11" s="12"/>
       <c r="I11" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="J11" s="13"/>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21" t="s">
-        <v>95</v>
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>26</v>
@@ -1435,7 +1427,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="13" t="s">
@@ -1443,14 +1435,14 @@
       </c>
       <c r="J12" s="13"/>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21" t="s">
-        <v>96</v>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>26</v>
@@ -1462,7 +1454,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="13" t="s">
@@ -1474,57 +1466,65 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21" t="s">
-        <v>97</v>
+      <c r="A14" s="18"/>
+      <c r="B14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="I14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="13"/>
+      <c r="J14" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="K14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="87" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
-      <c r="B15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>98</v>
+    <row r="15" spans="1:30" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>24</v>
@@ -1534,76 +1534,68 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>99</v>
+      <c r="A16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="21" t="s">
-        <v>100</v>
+      <c r="A17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H17" s="12"/>
       <c r="I17" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="J17" s="13"/>
       <c r="K17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="21" t="s">
-        <v>101</v>
+      <c r="A18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>34</v>
@@ -1615,7 +1607,7 @@
         <v>22</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="13" t="s">
@@ -1627,10 +1619,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="21" t="s">
-        <v>102</v>
+      <c r="A19" s="18"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>34</v>
@@ -1642,7 +1634,7 @@
         <v>22</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="13" t="s">
@@ -1654,10 +1646,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="21" t="s">
-        <v>103</v>
+      <c r="A20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>34</v>
@@ -1669,7 +1661,7 @@
         <v>22</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="13" t="s">
@@ -1677,14 +1669,14 @@
       </c>
       <c r="J20" s="13"/>
       <c r="K20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="21" t="s">
-        <v>104</v>
+      <c r="A21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>34</v>
@@ -1696,7 +1688,7 @@
         <v>22</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="13" t="s">
@@ -1704,14 +1696,14 @@
       </c>
       <c r="J21" s="13"/>
       <c r="K21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="21" t="s">
-        <v>105</v>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>34</v>
@@ -1723,7 +1715,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="13" t="s">
@@ -1731,74 +1723,74 @@
       </c>
       <c r="J22" s="13"/>
       <c r="K22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="17"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21" t="s">
-        <v>106</v>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="I23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="13"/>
+      <c r="J23" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="K23" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>107</v>
+      <c r="A24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="H24" s="12"/>
       <c r="I24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="J24" s="13"/>
       <c r="K24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="21" t="s">
-        <v>108</v>
+      <c r="A25" s="18"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="17" t="s">
+        <v>107</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>34</v>
@@ -1810,7 +1802,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="13" t="s">
@@ -1818,14 +1810,14 @@
       </c>
       <c r="J25" s="13"/>
       <c r="K25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="21" t="s">
-        <v>109</v>
+      <c r="A26" s="18"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>34</v>
@@ -1837,7 +1829,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="13" t="s">
@@ -1848,75 +1840,48 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21" t="s">
-        <v>110</v>
+    <row r="27" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A27" s="18"/>
+      <c r="B27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" s="12"/>
+        <v>42</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="I27" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J27" s="13"/>
+      <c r="J27" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="K27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
-      <c r="B28" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AD1" xr:uid="{2E8EC9D0-C91D-48DD-971A-EE0308A56452}"/>
   <mergeCells count="6">
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A16:A28"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A27"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B15:B22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>